<commit_message>
final, error in simulation
</commit_message>
<xml_diff>
--- a/input_nuts.xlsx
+++ b/input_nuts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a631459e6cf3f3cb/Uni/Master/2021_ss_decision-analysis/Agroforestry/Nuts_and_chicken/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="284" documentId="8_{B43E09B4-1D40-44D1-9E4B-3F328F31B02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B926B020-10F0-4FDC-BC90-B493DCE0F6C8}"/>
+  <xr:revisionPtr revIDLastSave="313" documentId="8_{B43E09B4-1D40-44D1-9E4B-3F328F31B02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB3A37FE-0BC2-46F1-AEA3-88EEFB2EDBD5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF154E54-C84F-4A74-9D1E-330DB1AEC478}"/>
+    <workbookView minimized="1" xWindow="7590" yWindow="0" windowWidth="17280" windowHeight="9030" xr2:uid="{FF154E54-C84F-4A74-9D1E-330DB1AEC478}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="103">
   <si>
     <t>variable</t>
   </si>
@@ -325,6 +325,24 @@
   </si>
   <si>
     <t>maintaining_trees_factor</t>
+  </si>
+  <si>
+    <t>tree_planting_hours_3</t>
+  </si>
+  <si>
+    <t>tree_planting_costs_3</t>
+  </si>
+  <si>
+    <t>maintaining_trees_3</t>
+  </si>
+  <si>
+    <t>mulch_h_3</t>
+  </si>
+  <si>
+    <t>tree_var_costs</t>
+  </si>
+  <si>
+    <t>Other tree costs</t>
   </si>
 </sst>
 </file>
@@ -679,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D257FCD1-4F27-4F6D-A626-0E17ED67B885}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,6 +1626,106 @@
         <v>81</v>
       </c>
     </row>
+    <row r="45" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="1">
+        <v>6</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="1">
+        <v>10</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="1">
+        <v>3700</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="1">
+        <v>4200</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="1">
+        <v>3</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="1">
+        <v>6</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="1">
+        <v>4</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="1">
+        <v>100</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="1">
+        <v>150</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>